<commit_message>
si corrijen varias cosas como :
traducciones de texto en Narratvias y sus opciones
textos prefijos para Cultura
correcciones a la data de cargue en IRA
</commit_message>
<xml_diff>
--- a/backend/data/CVF_data.xlsx
+++ b/backend/data/CVF_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDC8C70-202E-D240-BA2A-3C42A5343C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3BD58B-B579-A24D-89D7-A93F65276E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13760" yWindow="4820" windowWidth="37000" windowHeight="21920" xr2:uid="{CAEFDF89-58F6-428A-B484-A7386FFF6B3E}"/>
+    <workbookView xWindow="11980" yWindow="16080" windowWidth="48360" windowHeight="14280" activeTab="1" xr2:uid="{CAEFDF89-58F6-428A-B484-A7386FFF6B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Preguntas" sheetId="1" r:id="rId1"/>
@@ -69,24 +69,6 @@
     <t>Cohesión organizacional</t>
   </si>
   <si>
-    <t>Este colegio es:</t>
-  </si>
-  <si>
-    <t>El liderazgo en este colegio en general ejemplifica:</t>
-  </si>
-  <si>
-    <t>En este colegio, el estilo de manejo del equipo académico se caracteriza por:</t>
-  </si>
-  <si>
-    <t>Este colegio enfatiza:</t>
-  </si>
-  <si>
-    <t>Este colegio define el éxito sobre la base de:</t>
-  </si>
-  <si>
-    <t>Los elementos que le imprimen cohesión a este colegio son:</t>
-  </si>
-  <si>
     <t>…un lugar muy personal, como una familia extendida. Las persona comparten mucho de sí mismas.</t>
   </si>
   <si>
@@ -162,9 +144,6 @@
     <t xml:space="preserve">Dominant characteristics </t>
   </si>
   <si>
-    <t>The school is…</t>
-  </si>
-  <si>
     <t>…a very personal place, like an extended family. People share a lot of themselves.</t>
   </si>
   <si>
@@ -180,9 +159,6 @@
     <t>School cohesion</t>
   </si>
   <si>
-    <t>The elements that give the school cohesion are...</t>
-  </si>
-  <si>
     <t>…loyalty and mutual trust. The commitment to the organization is great.</t>
   </si>
   <si>
@@ -198,9 +174,6 @@
     <t>Organizational leadership</t>
   </si>
   <si>
-    <t>Leadership in the school in general exemplifies…</t>
-  </si>
-  <si>
     <t xml:space="preserve">…mentoring, facilitation, and care of the individual. </t>
   </si>
   <si>
@@ -216,9 +189,6 @@
     <t>Management of the academic team</t>
   </si>
   <si>
-    <t>At school, the management style of the academic team is characterized by...</t>
-  </si>
-  <si>
     <t>…teamwork, consensus, and participation.</t>
   </si>
   <si>
@@ -234,9 +204,6 @@
     <t>Strategic emphasis</t>
   </si>
   <si>
-    <t>The school emphasizes…</t>
-  </si>
-  <si>
     <t>…human development, trust, openness, and participation.</t>
   </si>
   <si>
@@ -261,9 +228,6 @@
     <t>…gaining market share and competing with other educational institutions.</t>
   </si>
   <si>
-    <t>This school defines success based on…</t>
-  </si>
-  <si>
     <t>…efficiency. Achieving targets, planning, and having defined budgets.</t>
   </si>
   <si>
@@ -295,6 +259,42 @@
   </si>
   <si>
     <t>Prefijo_es</t>
+  </si>
+  <si>
+    <t>Esta organización es:</t>
+  </si>
+  <si>
+    <t>El liderazgo en esta organización en general ejemplifica:</t>
+  </si>
+  <si>
+    <t>En esta organización, el estilo de manejo de la fuerza laboral se caracteriza por:</t>
+  </si>
+  <si>
+    <t>Los elementos que le imprimen cohesión a esta organización son:</t>
+  </si>
+  <si>
+    <t>This organization is:</t>
+  </si>
+  <si>
+    <t>Leadership in this organization generally exemplifies:</t>
+  </si>
+  <si>
+    <t>In this organization, the management style of the workforce is characterized by:</t>
+  </si>
+  <si>
+    <t>The elements that give cohesion to this organization are:</t>
+  </si>
+  <si>
+    <t>Esta organización enfatiza:</t>
+  </si>
+  <si>
+    <t>Esta organización define el éxito sobre la base de:</t>
+  </si>
+  <si>
+    <t>This organization emphasizes…</t>
+  </si>
+  <si>
+    <t>This organization defines success based on…</t>
   </si>
 </sst>
 </file>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA4DB68-6757-4D22-9604-C8A3AE113614}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -674,22 +674,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -706,10 +706,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -717,19 +717,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -737,19 +737,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -766,10 +766,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -777,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -786,10 +786,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -797,19 +797,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -817,19 +817,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -837,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -846,10 +846,10 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -857,7 +857,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -866,10 +866,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -877,19 +877,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -897,19 +897,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -917,7 +917,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -926,10 +926,10 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -937,7 +937,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -946,10 +946,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -957,19 +957,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -977,19 +977,19 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -997,7 +997,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -1006,10 +1006,10 @@
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1017,7 +1017,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -1026,10 +1026,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1037,19 +1037,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1057,19 +1057,19 @@
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1077,7 +1077,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -1086,10 +1086,10 @@
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1097,7 +1097,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1106,10 +1106,10 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1117,19 +1117,19 @@
         <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1137,19 +1137,19 @@
         <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1157,7 +1157,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1166,10 +1166,10 @@
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1181,30 +1181,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A749F17-7349-4715-89AD-9052387312AE}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
-    <col min="3" max="3" width="60" customWidth="1"/>
+    <col min="3" max="3" width="63.6640625" customWidth="1"/>
     <col min="4" max="4" width="62.83203125" customWidth="1"/>
+    <col min="5" max="5" width="64" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1212,13 +1213,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1226,13 +1227,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1240,13 +1241,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1254,13 +1255,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1268,13 +1269,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1282,13 +1283,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1312,10 +1313,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1331,7 +1332,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1339,7 +1340,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
se corrijen algunas palabras de Culture
</commit_message>
<xml_diff>
--- a/backend/data/CVF_data.xlsx
+++ b/backend/data/CVF_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3BD58B-B579-A24D-89D7-A93F65276E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5BDB35-5C74-EF47-96D4-8C0D0FF3B1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="16080" windowWidth="48360" windowHeight="14280" activeTab="1" xr2:uid="{CAEFDF89-58F6-428A-B484-A7386FFF6B3E}"/>
+    <workbookView xWindow="9400" yWindow="7300" windowWidth="36280" windowHeight="16480" xr2:uid="{CAEFDF89-58F6-428A-B484-A7386FFF6B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Preguntas" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>…lealtad y confianza mutua. El compromiso con la organización es grande.</t>
   </si>
   <si>
-    <t xml:space="preserve">...compromiso con la innovación y el desarrollo. Emfasis en posicionarse en prácticas (modelos, tecnología) de punta. </t>
-  </si>
-  <si>
     <t>…logros y cumplimiento de metas.</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>…prácticas educativas únicas y de punta. Es líder de productos e innovador.</t>
   </si>
   <si>
-    <t>…ganar participación en el mercado y competir con otras instituciones educativas.</t>
-  </si>
-  <si>
     <t>…eficiencia. Dependencia de cumplimiento, planeación y presupuestos definidos.</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>…unique and state-of-the-art educational practices. It is a leader and innovator.</t>
   </si>
   <si>
-    <t>…gaining market share and competing with other educational institutions.</t>
-  </si>
-  <si>
     <t>…efficiency. Achieving targets, planning, and having defined budgets.</t>
   </si>
   <si>
@@ -295,6 +286,15 @@
   </si>
   <si>
     <t>This organization defines success based on…</t>
+  </si>
+  <si>
+    <t>…ganar participación en el mercado y competir con otras compañias.</t>
+  </si>
+  <si>
+    <t>…gaining market share and competing with other companies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">...compromiso con la innovación y el desarrollo. Enfasis en posicionarse en prácticas (modelos, tecnología) de punta. </t>
   </si>
 </sst>
 </file>
@@ -361,9 +361,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -401,7 +401,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -507,7 +507,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -649,7 +649,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA4DB68-6757-4D22-9604-C8A3AE113614}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:E13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -674,22 +674,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -709,7 +709,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -717,19 +717,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -737,19 +737,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -769,7 +769,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -777,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -789,7 +789,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -797,19 +797,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -817,19 +817,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -837,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -849,7 +849,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -857,7 +857,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -869,7 +869,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -877,19 +877,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -897,19 +897,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -917,7 +917,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -929,7 +929,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -937,7 +937,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -949,7 +949,7 @@
         <v>22</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -957,19 +957,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -977,19 +977,19 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -997,7 +997,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -1006,10 +1006,10 @@
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1017,7 +1017,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -1026,10 +1026,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1037,19 +1037,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1057,19 +1057,19 @@
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1077,7 +1077,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -1086,10 +1086,10 @@
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1097,7 +1097,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1106,10 +1106,10 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1117,19 +1117,19 @@
         <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1137,19 +1137,19 @@
         <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1157,7 +1157,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1166,10 +1166,10 @@
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1181,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A749F17-7349-4715-89AD-9052387312AE}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1196,16 +1196,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1213,13 +1213,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1227,13 +1227,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1241,13 +1241,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1255,13 +1255,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1269,13 +1269,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1283,13 +1283,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1313,10 +1313,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1332,7 +1332,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1340,7 +1340,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>